<commit_message>
update cross list file
</commit_message>
<xml_diff>
--- a/pnsearch/Inductor Cross List.xlsx
+++ b/pnsearch/Inductor Cross List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13726" uniqueCount="2411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14144" uniqueCount="2411">
   <si>
     <t>Würth PN</t>
   </si>
@@ -7614,7 +7614,7 @@
   <dimension ref="A1:Q3428"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3342" workbookViewId="0">
-      <selection activeCell="D3342" sqref="D3342"/>
+      <selection activeCell="D3343" sqref="D3343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59969,6 +59969,9 @@
       <c r="C3000" s="1" t="s">
         <v>1592</v>
       </c>
+      <c r="D3000" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3000" s="1" t="s">
         <v>1930</v>
       </c>
@@ -59983,6 +59986,9 @@
       <c r="C3001" s="1" t="s">
         <v>1597</v>
       </c>
+      <c r="D3001" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3001" s="1" t="s">
         <v>1931</v>
       </c>
@@ -59997,6 +60003,9 @@
       <c r="C3002" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3002" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3002" s="1" t="s">
         <v>10</v>
       </c>
@@ -60011,6 +60020,9 @@
       <c r="C3003" s="1" t="s">
         <v>1597</v>
       </c>
+      <c r="D3003" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3003" s="1" t="s">
         <v>1932</v>
       </c>
@@ -60025,6 +60037,9 @@
       <c r="C3004" s="1" t="s">
         <v>1597</v>
       </c>
+      <c r="D3004" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3004" s="1" t="s">
         <v>1933</v>
       </c>
@@ -60039,6 +60054,9 @@
       <c r="C3005" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="D3005" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3005" s="1" t="s">
         <v>1934</v>
       </c>
@@ -60053,6 +60071,9 @@
       <c r="C3006" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="D3006" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3006" s="1" t="s">
         <v>1935</v>
       </c>
@@ -60068,6 +60089,9 @@
       <c r="C3007" s="1" t="s">
         <v>1905</v>
       </c>
+      <c r="D3007" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3007" s="1" t="s">
         <v>1936</v>
       </c>
@@ -60082,6 +60106,9 @@
       <c r="C3008" s="1" t="s">
         <v>1336</v>
       </c>
+      <c r="D3008" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3008" s="1" t="s">
         <v>1937</v>
       </c>
@@ -60097,6 +60124,9 @@
       <c r="C3009" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3009" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3009" s="1" t="s">
         <v>1938</v>
       </c>
@@ -60112,6 +60142,9 @@
       <c r="C3010" s="1" t="s">
         <v>1940</v>
       </c>
+      <c r="D3010" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3010" s="1" t="s">
         <v>1939</v>
       </c>
@@ -60126,6 +60159,9 @@
       <c r="C3011" s="1" t="s">
         <v>1942</v>
       </c>
+      <c r="D3011" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3011" s="1" t="s">
         <v>1941</v>
       </c>
@@ -60140,6 +60176,9 @@
       <c r="C3012" s="1" t="s">
         <v>1944</v>
       </c>
+      <c r="D3012" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3012" s="1" t="s">
         <v>1943</v>
       </c>
@@ -60154,6 +60193,9 @@
       <c r="C3013" s="1" t="s">
         <v>1946</v>
       </c>
+      <c r="D3013" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3013" s="1" t="s">
         <v>1945</v>
       </c>
@@ -60168,6 +60210,9 @@
       <c r="C3014" s="1" t="s">
         <v>1948</v>
       </c>
+      <c r="D3014" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3014" s="1" t="s">
         <v>1609</v>
       </c>
@@ -60182,6 +60227,9 @@
       <c r="C3015" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3015" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3015" s="1" t="s">
         <v>1949</v>
       </c>
@@ -60197,6 +60245,9 @@
       <c r="C3016" s="1" t="s">
         <v>1950</v>
       </c>
+      <c r="D3016" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3016" s="1" t="s">
         <v>1613</v>
       </c>
@@ -60211,6 +60262,9 @@
       <c r="C3017" s="1" t="s">
         <v>1952</v>
       </c>
+      <c r="D3017" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3017" s="1" t="s">
         <v>1951</v>
       </c>
@@ -60225,6 +60279,9 @@
       <c r="C3018" s="1" t="s">
         <v>1954</v>
       </c>
+      <c r="D3018" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3018" s="1" t="s">
         <v>1953</v>
       </c>
@@ -60239,6 +60296,9 @@
       <c r="C3019" s="1" t="s">
         <v>1955</v>
       </c>
+      <c r="D3019" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3019" s="1" t="s">
         <v>1615</v>
       </c>
@@ -60253,6 +60313,9 @@
       <c r="C3020" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3020" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3020" s="1" t="s">
         <v>10</v>
       </c>
@@ -60267,6 +60330,9 @@
       <c r="C3021" s="1" t="s">
         <v>1957</v>
       </c>
+      <c r="D3021" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3021" s="1" t="s">
         <v>1956</v>
       </c>
@@ -60281,6 +60347,9 @@
       <c r="C3022" s="1" t="s">
         <v>1950</v>
       </c>
+      <c r="D3022" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3022" s="1" t="s">
         <v>1618</v>
       </c>
@@ -60295,6 +60364,9 @@
       <c r="C3023" s="1" t="s">
         <v>1959</v>
       </c>
+      <c r="D3023" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3023" s="1" t="s">
         <v>1958</v>
       </c>
@@ -60309,6 +60381,9 @@
       <c r="C3024" s="1" t="s">
         <v>1962</v>
       </c>
+      <c r="D3024" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3024" s="1" t="s">
         <v>1960</v>
       </c>
@@ -60324,6 +60399,9 @@
       <c r="C3025" s="1" t="s">
         <v>1963</v>
       </c>
+      <c r="D3025" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3025" s="1" t="s">
         <v>1620</v>
       </c>
@@ -60339,6 +60417,9 @@
       <c r="C3026" s="1" t="s">
         <v>1965</v>
       </c>
+      <c r="D3026" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3026" s="1" t="s">
         <v>1964</v>
       </c>
@@ -60354,6 +60435,9 @@
       <c r="C3027" s="1" t="s">
         <v>1966</v>
       </c>
+      <c r="D3027" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3027" s="1" t="s">
         <v>1624</v>
       </c>
@@ -60368,6 +60452,9 @@
       <c r="C3028" s="1" t="s">
         <v>1967</v>
       </c>
+      <c r="D3028" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3028" s="1" t="s">
         <v>1627</v>
       </c>
@@ -60382,6 +60469,9 @@
       <c r="C3029" s="1" t="s">
         <v>1968</v>
       </c>
+      <c r="D3029" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3029" s="1" t="s">
         <v>1629</v>
       </c>
@@ -60396,6 +60486,9 @@
       <c r="C3030" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3030" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3030" s="1" t="s">
         <v>1969</v>
       </c>
@@ -60410,6 +60503,9 @@
       <c r="C3031" s="1" t="s">
         <v>1576</v>
       </c>
+      <c r="D3031" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3031" s="1" t="s">
         <v>1970</v>
       </c>
@@ -60424,6 +60520,9 @@
       <c r="C3032" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3032" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3032" s="1" t="s">
         <v>10</v>
       </c>
@@ -60438,6 +60537,9 @@
       <c r="C3033" s="1" t="s">
         <v>1972</v>
       </c>
+      <c r="D3033" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3033" s="1" t="s">
         <v>1971</v>
       </c>
@@ -60452,6 +60554,9 @@
       <c r="C3034" s="1" t="s">
         <v>1582</v>
       </c>
+      <c r="D3034" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3034" s="1" t="s">
         <v>978</v>
       </c>
@@ -60467,6 +60572,9 @@
       <c r="C3035" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3035" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3035" s="1" t="s">
         <v>10</v>
       </c>
@@ -60481,6 +60589,9 @@
       <c r="C3036" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3036" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3036" s="1" t="s">
         <v>10</v>
       </c>
@@ -60495,6 +60606,9 @@
       <c r="C3037" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3037" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3037" s="1" t="s">
         <v>1973</v>
       </c>
@@ -60510,6 +60624,9 @@
       <c r="C3038" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3038" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3038" s="1" t="s">
         <v>10</v>
       </c>
@@ -60524,6 +60641,9 @@
       <c r="C3039" s="1" t="s">
         <v>1565</v>
       </c>
+      <c r="D3039" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3039" s="1" t="s">
         <v>1974</v>
       </c>
@@ -60538,6 +60658,9 @@
       <c r="C3040" s="1" t="s">
         <v>1588</v>
       </c>
+      <c r="D3040" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3040" s="1" t="s">
         <v>1975</v>
       </c>
@@ -60552,6 +60675,9 @@
       <c r="C3041" s="1" t="s">
         <v>1592</v>
       </c>
+      <c r="D3041" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3041" s="1" t="s">
         <v>1976</v>
       </c>
@@ -60566,6 +60692,9 @@
       <c r="C3042" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3042" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3042" s="1" t="s">
         <v>10</v>
       </c>
@@ -60581,6 +60710,9 @@
       <c r="C3043" s="1" t="s">
         <v>1568</v>
       </c>
+      <c r="D3043" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3043" s="1" t="s">
         <v>1977</v>
       </c>
@@ -60596,6 +60728,9 @@
       <c r="C3044" s="1" t="s">
         <v>1592</v>
       </c>
+      <c r="D3044" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3044" s="1" t="s">
         <v>973</v>
       </c>
@@ -60610,6 +60745,9 @@
       <c r="C3045" s="1" t="s">
         <v>1597</v>
       </c>
+      <c r="D3045" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3045" s="1" t="s">
         <v>1978</v>
       </c>
@@ -60624,6 +60762,9 @@
       <c r="C3046" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3046" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3046" s="1" t="s">
         <v>10</v>
       </c>
@@ -60638,6 +60779,9 @@
       <c r="C3047" s="1" t="s">
         <v>1573</v>
       </c>
+      <c r="D3047" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3047" s="1" t="s">
         <v>1979</v>
       </c>
@@ -60652,6 +60796,9 @@
       <c r="C3048" s="1" t="s">
         <v>1597</v>
       </c>
+      <c r="D3048" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3048" s="1" t="s">
         <v>1980</v>
       </c>
@@ -60666,6 +60813,9 @@
       <c r="C3049" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3049" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3049" s="1" t="s">
         <v>1981</v>
       </c>
@@ -60680,6 +60830,9 @@
       <c r="C3050" s="1" t="s">
         <v>1920</v>
       </c>
+      <c r="D3050" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3050" s="1" t="s">
         <v>1982</v>
       </c>
@@ -60694,6 +60847,9 @@
       <c r="C3051" s="1" t="s">
         <v>1905</v>
       </c>
+      <c r="D3051" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3051" s="1" t="s">
         <v>1983</v>
       </c>
@@ -60708,6 +60864,9 @@
       <c r="C3052" s="1" t="s">
         <v>1905</v>
       </c>
+      <c r="D3052" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3052" s="1" t="s">
         <v>1984</v>
       </c>
@@ -60722,6 +60881,9 @@
       <c r="C3053" s="1" t="s">
         <v>1336</v>
       </c>
+      <c r="D3053" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3053" s="1" t="s">
         <v>1985</v>
       </c>
@@ -60736,6 +60898,9 @@
       <c r="C3054" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3054" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3054" s="1" t="s">
         <v>10</v>
       </c>
@@ -60750,6 +60915,9 @@
       <c r="C3055" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3055" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3055" s="1" t="s">
         <v>10</v>
       </c>
@@ -60764,6 +60932,9 @@
       <c r="C3056" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3056" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3056" s="1" t="s">
         <v>10</v>
       </c>
@@ -60778,6 +60949,9 @@
       <c r="C3057" s="1" t="s">
         <v>1989</v>
       </c>
+      <c r="D3057" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3057" s="1" t="s">
         <v>1988</v>
       </c>
@@ -60792,6 +60966,9 @@
       <c r="C3058" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3058" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3058" s="1" t="s">
         <v>10</v>
       </c>
@@ -60806,6 +60983,9 @@
       <c r="C3059" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3059" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3059" s="1" t="s">
         <v>1990</v>
       </c>
@@ -60820,6 +61000,9 @@
       <c r="C3060" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3060" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3060" s="1" t="s">
         <v>1992</v>
       </c>
@@ -60834,6 +61017,9 @@
       <c r="C3061" s="1" t="s">
         <v>1994</v>
       </c>
+      <c r="D3061" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3061" s="1" t="s">
         <v>1993</v>
       </c>
@@ -60848,6 +61034,9 @@
       <c r="C3062" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3062" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3062" s="1" t="s">
         <v>1995</v>
       </c>
@@ -60862,6 +61051,9 @@
       <c r="C3063" s="1" t="s">
         <v>1998</v>
       </c>
+      <c r="D3063" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3063" s="1" t="s">
         <v>1997</v>
       </c>
@@ -60876,6 +61068,9 @@
       <c r="C3064" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3064" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3064" s="1" t="s">
         <v>981</v>
       </c>
@@ -60890,6 +61085,9 @@
       <c r="C3065" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3065" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3065" s="1" t="s">
         <v>1999</v>
       </c>
@@ -60904,6 +61102,9 @@
       <c r="C3066" s="1" t="s">
         <v>2002</v>
       </c>
+      <c r="D3066" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3066" s="1" t="s">
         <v>2000</v>
       </c>
@@ -60919,6 +61120,9 @@
       <c r="C3067" s="1" t="s">
         <v>1363</v>
       </c>
+      <c r="D3067" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3067" s="1" t="s">
         <v>2003</v>
       </c>
@@ -60934,6 +61138,9 @@
       <c r="C3068" s="1" t="s">
         <v>1363</v>
       </c>
+      <c r="D3068" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3068" s="1" t="s">
         <v>2004</v>
       </c>
@@ -60949,6 +61156,9 @@
       <c r="C3069" s="1" t="s">
         <v>2007</v>
       </c>
+      <c r="D3069" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3069" s="1" t="s">
         <v>2005</v>
       </c>
@@ -60965,6 +61175,9 @@
       <c r="C3070" s="1" t="s">
         <v>2008</v>
       </c>
+      <c r="D3070" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3070" s="1" t="s">
         <v>984</v>
       </c>
@@ -60979,6 +61192,9 @@
       <c r="C3071" s="1" t="s">
         <v>2010</v>
       </c>
+      <c r="D3071" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3071" s="1" t="s">
         <v>2009</v>
       </c>
@@ -60994,6 +61210,9 @@
       <c r="C3072" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3072" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3072" s="1" t="s">
         <v>2011</v>
       </c>
@@ -61009,6 +61228,9 @@
       <c r="C3073" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3073" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3073" s="1" t="s">
         <v>2012</v>
       </c>
@@ -61024,6 +61246,9 @@
       <c r="C3074" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3074" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3074" s="1" t="s">
         <v>2013</v>
       </c>
@@ -61040,6 +61265,9 @@
       <c r="C3075" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3075" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3075" s="1" t="s">
         <v>2014</v>
       </c>
@@ -61055,6 +61283,9 @@
       <c r="C3076" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3076" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3076" s="1" t="s">
         <v>2015</v>
       </c>
@@ -61069,6 +61300,9 @@
       <c r="C3077" s="1" t="s">
         <v>1994</v>
       </c>
+      <c r="D3077" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3077" s="1" t="s">
         <v>1956</v>
       </c>
@@ -61083,6 +61317,9 @@
       <c r="C3078" s="1" t="s">
         <v>1998</v>
       </c>
+      <c r="D3078" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3078" s="1" t="s">
         <v>2016</v>
       </c>
@@ -61097,6 +61334,9 @@
       <c r="C3079" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3079" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3079" s="1" t="s">
         <v>2017</v>
       </c>
@@ -61111,6 +61351,9 @@
       <c r="C3080" s="1" t="s">
         <v>1998</v>
       </c>
+      <c r="D3080" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3080" s="1" t="s">
         <v>2018</v>
       </c>
@@ -61125,6 +61368,9 @@
       <c r="C3081" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3081" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3081" s="1" t="s">
         <v>2019</v>
       </c>
@@ -61139,6 +61385,9 @@
       <c r="C3082" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3082" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3082" s="1" t="s">
         <v>2020</v>
       </c>
@@ -61153,6 +61402,9 @@
       <c r="C3083" s="1" t="s">
         <v>2002</v>
       </c>
+      <c r="D3083" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3083" s="1" t="s">
         <v>1964</v>
       </c>
@@ -61167,6 +61419,9 @@
       <c r="C3084" s="1" t="s">
         <v>1363</v>
       </c>
+      <c r="D3084" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3084" s="1" t="s">
         <v>2021</v>
       </c>
@@ -61181,6 +61436,9 @@
       <c r="C3085" s="1" t="s">
         <v>2007</v>
       </c>
+      <c r="D3085" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3085" s="1" t="s">
         <v>2022</v>
       </c>
@@ -61196,6 +61454,9 @@
       <c r="C3086" s="1" t="s">
         <v>1366</v>
       </c>
+      <c r="D3086" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3086" s="1" t="s">
         <v>2023</v>
       </c>
@@ -61210,6 +61471,9 @@
       <c r="C3087" s="1" t="s">
         <v>2008</v>
       </c>
+      <c r="D3087" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3087" s="1" t="s">
         <v>1969</v>
       </c>
@@ -61224,6 +61488,9 @@
       <c r="C3088" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3088" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3088" s="1" t="s">
         <v>10</v>
       </c>
@@ -61238,6 +61505,9 @@
       <c r="C3089" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3089" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3089" s="1" t="s">
         <v>2025</v>
       </c>
@@ -61253,6 +61523,9 @@
       <c r="C3090" s="1" t="s">
         <v>1989</v>
       </c>
+      <c r="D3090" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3090" s="1" t="s">
         <v>2027</v>
       </c>
@@ -61267,6 +61540,9 @@
       <c r="C3091" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3091" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3091" s="1" t="s">
         <v>2029</v>
       </c>
@@ -61281,6 +61557,9 @@
       <c r="C3092" s="1" t="s">
         <v>1994</v>
       </c>
+      <c r="D3092" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3092" s="1" t="s">
         <v>2030</v>
       </c>
@@ -61295,6 +61574,9 @@
       <c r="C3093" s="1" t="s">
         <v>1998</v>
       </c>
+      <c r="D3093" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3093" s="1" t="s">
         <v>2031</v>
       </c>
@@ -61309,6 +61591,9 @@
       <c r="C3094" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3094" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3094" s="1" t="s">
         <v>2032</v>
       </c>
@@ -61325,6 +61610,9 @@
       <c r="C3095" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3095" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3095" s="1" t="s">
         <v>445</v>
       </c>
@@ -61339,6 +61627,9 @@
       <c r="C3096" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3096" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3096" s="1" t="s">
         <v>2033</v>
       </c>
@@ -61387,6 +61678,9 @@
       <c r="C3099" s="1" t="s">
         <v>1366</v>
       </c>
+      <c r="D3099" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3099" s="1" t="s">
         <v>2036</v>
       </c>
@@ -61401,6 +61695,9 @@
       <c r="C3100" s="1" t="s">
         <v>1375</v>
       </c>
+      <c r="D3100" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3100" s="1" t="s">
         <v>2037</v>
       </c>
@@ -61415,6 +61712,9 @@
       <c r="C3101" s="1" t="s">
         <v>2038</v>
       </c>
+      <c r="D3101" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3101" s="1" t="s">
         <v>445</v>
       </c>
@@ -61429,6 +61729,9 @@
       <c r="C3102" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="D3102" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3102" s="1" t="s">
         <v>2039</v>
       </c>
@@ -61443,6 +61746,9 @@
       <c r="C3103" s="1" t="s">
         <v>1377</v>
       </c>
+      <c r="D3103" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3103" s="1" t="s">
         <v>2040</v>
       </c>
@@ -61457,6 +61763,9 @@
       <c r="C3104" s="1" t="s">
         <v>2042</v>
       </c>
+      <c r="D3104" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3104" s="1" t="s">
         <v>2041</v>
       </c>
@@ -61471,6 +61780,9 @@
       <c r="C3105" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3105" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3105" s="1" t="s">
         <v>2043</v>
       </c>
@@ -61485,6 +61797,9 @@
       <c r="C3106" s="1" t="s">
         <v>2045</v>
       </c>
+      <c r="D3106" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3106" s="1" t="s">
         <v>2044</v>
       </c>
@@ -61499,6 +61814,9 @@
       <c r="C3107" s="1" t="s">
         <v>2048</v>
       </c>
+      <c r="D3107" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3107" s="1" t="s">
         <v>2046</v>
       </c>
@@ -61513,6 +61831,9 @@
       <c r="C3108" s="1" t="s">
         <v>1989</v>
       </c>
+      <c r="D3108" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3108" s="1" t="s">
         <v>2049</v>
       </c>
@@ -61527,6 +61848,9 @@
       <c r="C3109" s="1" t="s">
         <v>1991</v>
       </c>
+      <c r="D3109" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3109" s="1" t="s">
         <v>2050</v>
       </c>
@@ -61541,6 +61865,9 @@
       <c r="C3110" s="1" t="s">
         <v>1996</v>
       </c>
+      <c r="D3110" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3110" s="1" t="s">
         <v>2051</v>
       </c>
@@ -61556,6 +61883,9 @@
       <c r="C3111" s="1" t="s">
         <v>2002</v>
       </c>
+      <c r="D3111" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3111" s="1" t="s">
         <v>2053</v>
       </c>
@@ -61570,6 +61900,9 @@
       <c r="C3112" s="1" t="s">
         <v>1363</v>
       </c>
+      <c r="D3112" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3112" s="1" t="s">
         <v>2055</v>
       </c>
@@ -61586,6 +61919,9 @@
       <c r="C3113" s="1" t="s">
         <v>2007</v>
       </c>
+      <c r="D3113" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3113" s="1" t="s">
         <v>2057</v>
       </c>
@@ -61601,6 +61937,9 @@
       <c r="C3114" s="1" t="s">
         <v>1366</v>
       </c>
+      <c r="D3114" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3114" s="1" t="s">
         <v>2058</v>
       </c>
@@ -61616,6 +61955,9 @@
       <c r="C3115" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3115" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3115" s="1" t="s">
         <v>2060</v>
       </c>
@@ -61631,6 +61973,9 @@
       <c r="C3116" s="1" t="s">
         <v>2038</v>
       </c>
+      <c r="D3116" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3116" s="1" t="s">
         <v>2062</v>
       </c>
@@ -61645,6 +61990,9 @@
       <c r="C3117" s="1" t="s">
         <v>1376</v>
       </c>
+      <c r="D3117" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3117" s="1" t="s">
         <v>2063</v>
       </c>
@@ -61659,6 +62007,9 @@
       <c r="C3118" s="1" t="s">
         <v>1377</v>
       </c>
+      <c r="D3118" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3118" s="1" t="s">
         <v>2064</v>
       </c>
@@ -61673,6 +62024,9 @@
       <c r="C3119" s="1" t="s">
         <v>2042</v>
       </c>
+      <c r="D3119" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3119" s="1" t="s">
         <v>2065</v>
       </c>
@@ -61688,6 +62042,9 @@
       <c r="C3120" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3120" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3120" s="1" t="s">
         <v>2067</v>
       </c>
@@ -61702,6 +62059,9 @@
       <c r="C3121" s="1" t="s">
         <v>2045</v>
       </c>
+      <c r="D3121" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3121" s="1" t="s">
         <v>2068</v>
       </c>
@@ -61716,6 +62076,9 @@
       <c r="C3122" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3122" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3122" s="1" t="s">
         <v>10</v>
       </c>
@@ -61730,6 +62093,9 @@
       <c r="C3123" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3123" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3123" s="1" t="s">
         <v>10</v>
       </c>
@@ -61745,6 +62111,9 @@
       <c r="C3124" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3124" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3124" s="1" t="s">
         <v>445</v>
       </c>
@@ -61759,6 +62128,9 @@
       <c r="C3125" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3125" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3125" s="1" t="s">
         <v>445</v>
       </c>
@@ -61774,6 +62146,9 @@
       <c r="C3126" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3126" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3126" s="1" t="s">
         <v>445</v>
       </c>
@@ -61788,6 +62163,9 @@
       <c r="C3127" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3127" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3127" s="1" t="s">
         <v>445</v>
       </c>
@@ -61802,6 +62180,9 @@
       <c r="C3128" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3128" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3128" s="1" t="s">
         <v>445</v>
       </c>
@@ -61817,6 +62198,9 @@
       <c r="C3129" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3129" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3129" s="1" t="s">
         <v>445</v>
       </c>
@@ -61832,6 +62216,9 @@
       <c r="C3130" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3130" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3130" s="1" t="s">
         <v>445</v>
       </c>
@@ -61847,6 +62234,9 @@
       <c r="C3131" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3131" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3131" s="1" t="s">
         <v>445</v>
       </c>
@@ -61861,6 +62251,9 @@
       <c r="C3132" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3132" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3132" s="1" t="s">
         <v>10</v>
       </c>
@@ -61875,6 +62268,9 @@
       <c r="C3133" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3133" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3133" s="1" t="s">
         <v>10</v>
       </c>
@@ -61890,6 +62286,9 @@
       <c r="C3134" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3134" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3134" s="1" t="s">
         <v>10</v>
       </c>
@@ -61904,6 +62303,9 @@
       <c r="C3135" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3135" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3135" s="1" t="s">
         <v>10</v>
       </c>
@@ -61918,6 +62320,9 @@
       <c r="C3136" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3136" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3136" s="1" t="s">
         <v>10</v>
       </c>
@@ -61932,6 +62337,9 @@
       <c r="C3137" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3137" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3137" s="1" t="s">
         <v>10</v>
       </c>
@@ -61946,6 +62354,9 @@
       <c r="C3138" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3138" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3138" s="1" t="s">
         <v>10</v>
       </c>
@@ -61960,6 +62371,9 @@
       <c r="C3139" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3139" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3139" s="1" t="s">
         <v>10</v>
       </c>
@@ -61974,6 +62388,9 @@
       <c r="C3140" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3140" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3140" s="1" t="s">
         <v>10</v>
       </c>
@@ -61988,6 +62405,9 @@
       <c r="C3141" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3141" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3141" s="1" t="s">
         <v>2070</v>
       </c>
@@ -62002,6 +62422,9 @@
       <c r="C3142" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3142" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3142" s="1" t="s">
         <v>10</v>
       </c>
@@ -62016,6 +62439,9 @@
       <c r="C3143" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3143" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3143" s="1" t="s">
         <v>10</v>
       </c>
@@ -62030,6 +62456,9 @@
       <c r="C3144" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3144" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3144" s="1" t="s">
         <v>10</v>
       </c>
@@ -62044,6 +62473,9 @@
       <c r="C3145" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3145" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3145" s="1" t="s">
         <v>10</v>
       </c>
@@ -62059,6 +62491,9 @@
       <c r="C3146" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3146" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3146" s="1" t="s">
         <v>10</v>
       </c>
@@ -62074,6 +62509,9 @@
       <c r="C3147" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3147" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3147" s="1" t="s">
         <v>10</v>
       </c>
@@ -62088,6 +62526,9 @@
       <c r="C3148" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3148" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3148" s="1" t="s">
         <v>2071</v>
       </c>
@@ -62191,6 +62632,9 @@
       <c r="C3154" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3154" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3154" s="1" t="s">
         <v>2080</v>
       </c>
@@ -62205,6 +62649,9 @@
       <c r="C3155" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3155" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3155" s="1" t="s">
         <v>2081</v>
       </c>
@@ -62219,6 +62666,9 @@
       <c r="C3156" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3156" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3156" s="1" t="s">
         <v>2083</v>
       </c>
@@ -62233,6 +62683,9 @@
       <c r="C3157" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3157" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3157" s="1" t="s">
         <v>2084</v>
       </c>
@@ -62247,6 +62700,9 @@
       <c r="C3158" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3158" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3158" s="1" t="s">
         <v>2086</v>
       </c>
@@ -62261,6 +62717,9 @@
       <c r="C3159" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3159" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3159" s="1" t="s">
         <v>2088</v>
       </c>
@@ -62275,6 +62734,9 @@
       <c r="C3160" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3160" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3160" s="1" t="s">
         <v>2090</v>
       </c>
@@ -62289,6 +62751,9 @@
       <c r="C3161" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3161" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3161" s="1" t="s">
         <v>2091</v>
       </c>
@@ -62303,6 +62768,9 @@
       <c r="C3162" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3162" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3162" s="1" t="s">
         <v>2092</v>
       </c>
@@ -62317,6 +62785,9 @@
       <c r="C3163" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3163" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3163" s="1" t="s">
         <v>2093</v>
       </c>
@@ -62331,6 +62802,9 @@
       <c r="C3164" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3164" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3164" s="1" t="s">
         <v>2094</v>
       </c>
@@ -62345,6 +62819,9 @@
       <c r="C3165" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3165" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3165" s="1" t="s">
         <v>2096</v>
       </c>
@@ -62360,6 +62837,9 @@
       <c r="C3166" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3166" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3166" s="1" t="s">
         <v>2097</v>
       </c>
@@ -62376,6 +62856,9 @@
       <c r="C3167" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3167" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3167" s="1" t="s">
         <v>2099</v>
       </c>
@@ -62391,6 +62874,9 @@
       <c r="C3168" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3168" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3168" s="1" t="s">
         <v>2100</v>
       </c>
@@ -62405,6 +62891,9 @@
       <c r="C3169" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3169" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3169" s="1" t="s">
         <v>2101</v>
       </c>
@@ -62419,6 +62908,9 @@
       <c r="C3170" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3170" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3170" s="1" t="s">
         <v>2102</v>
       </c>
@@ -62433,6 +62925,9 @@
       <c r="C3171" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3171" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3171" s="1" t="s">
         <v>2103</v>
       </c>
@@ -62447,6 +62942,9 @@
       <c r="C3172" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3172" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3172" s="1" t="s">
         <v>2105</v>
       </c>
@@ -62461,6 +62959,9 @@
       <c r="C3173" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3173" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3173" s="1" t="s">
         <v>2106</v>
       </c>
@@ -62475,6 +62976,9 @@
       <c r="C3174" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3174" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3174" s="1" t="s">
         <v>2108</v>
       </c>
@@ -62489,6 +62993,9 @@
       <c r="C3175" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3175" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3175" s="1" t="s">
         <v>2109</v>
       </c>
@@ -62503,6 +63010,9 @@
       <c r="C3176" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3176" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3176" s="1" t="s">
         <v>2111</v>
       </c>
@@ -62517,6 +63027,9 @@
       <c r="C3177" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3177" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3177" s="1" t="s">
         <v>1402</v>
       </c>
@@ -62531,6 +63044,9 @@
       <c r="C3178" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3178" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3178" s="1" t="s">
         <v>1405</v>
       </c>
@@ -62545,6 +63061,9 @@
       <c r="C3179" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3179" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3179" s="1" t="s">
         <v>10</v>
       </c>
@@ -62559,6 +63078,9 @@
       <c r="C3180" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3180" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3180" s="1" t="s">
         <v>2114</v>
       </c>
@@ -62573,6 +63095,9 @@
       <c r="C3181" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3181" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3181" s="1" t="s">
         <v>10</v>
       </c>
@@ -62587,6 +63112,9 @@
       <c r="C3182" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3182" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3182" s="1" t="s">
         <v>10</v>
       </c>
@@ -62602,6 +63130,9 @@
       <c r="C3183" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3183" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3183" s="1" t="s">
         <v>10</v>
       </c>
@@ -62616,6 +63147,9 @@
       <c r="C3184" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3184" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3184" s="1" t="s">
         <v>10</v>
       </c>
@@ -62630,6 +63164,9 @@
       <c r="C3185" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3185" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3185" s="1" t="s">
         <v>10</v>
       </c>
@@ -62644,6 +63181,9 @@
       <c r="C3186" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3186" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3186" s="1" t="s">
         <v>10</v>
       </c>
@@ -62658,6 +63198,9 @@
       <c r="C3187" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3187" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3187" s="1" t="s">
         <v>10</v>
       </c>
@@ -62673,6 +63216,9 @@
       <c r="C3188" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3188" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3188" s="1" t="s">
         <v>10</v>
       </c>
@@ -62688,6 +63234,9 @@
       <c r="C3189" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3189" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3189" s="1" t="s">
         <v>2116</v>
       </c>
@@ -62703,6 +63252,9 @@
       <c r="C3190" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3190" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3190" s="1" t="s">
         <v>10</v>
       </c>
@@ -62718,6 +63270,9 @@
       <c r="C3191" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3191" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3191" s="1" t="s">
         <v>10</v>
       </c>
@@ -62733,6 +63288,9 @@
       <c r="C3192" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3192" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3192" s="1" t="s">
         <v>10</v>
       </c>
@@ -62747,6 +63305,9 @@
       <c r="C3193" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3193" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3193" s="1" t="s">
         <v>2117</v>
       </c>
@@ -62762,6 +63323,9 @@
       <c r="C3194" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3194" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3194" s="1" t="s">
         <v>10</v>
       </c>
@@ -62777,6 +63341,9 @@
       <c r="C3195" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3195" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3195" s="1" t="s">
         <v>10</v>
       </c>
@@ -62792,6 +63359,9 @@
       <c r="C3196" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="D3196" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3196" s="1" t="s">
         <v>1459</v>
       </c>
@@ -62806,6 +63376,9 @@
       <c r="C3197" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3197" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3197" s="1" t="s">
         <v>1460</v>
       </c>
@@ -62820,6 +63393,9 @@
       <c r="C3198" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3198" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3198" s="1" t="s">
         <v>1461</v>
       </c>
@@ -62834,6 +63410,9 @@
       <c r="C3199" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="D3199" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3199" s="1" t="s">
         <v>1462</v>
       </c>
@@ -62848,6 +63427,9 @@
       <c r="C3200" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="D3200" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3200" s="1" t="s">
         <v>1463</v>
       </c>
@@ -62862,6 +63444,9 @@
       <c r="C3201" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="D3201" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3201" s="1" t="s">
         <v>1464</v>
       </c>
@@ -62876,6 +63461,9 @@
       <c r="C3202" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="D3202" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3202" s="1" t="s">
         <v>1465</v>
       </c>
@@ -62890,6 +63478,9 @@
       <c r="C3203" s="1" t="s">
         <v>1500</v>
       </c>
+      <c r="D3203" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3203" s="1" t="s">
         <v>2119</v>
       </c>
@@ -62904,6 +63495,9 @@
       <c r="C3204" s="1" t="s">
         <v>1524</v>
       </c>
+      <c r="D3204" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3204" s="1" t="s">
         <v>2121</v>
       </c>
@@ -62918,6 +63512,9 @@
       <c r="C3205" s="1" t="s">
         <v>1541</v>
       </c>
+      <c r="D3205" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3205" s="1" t="s">
         <v>2123</v>
       </c>
@@ -62932,6 +63529,9 @@
       <c r="C3206" s="1" t="s">
         <v>1312</v>
       </c>
+      <c r="D3206" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3206" s="1" t="s">
         <v>2125</v>
       </c>
@@ -62946,6 +63546,9 @@
       <c r="C3207" s="1" t="s">
         <v>1573</v>
       </c>
+      <c r="D3207" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3207" s="1" t="s">
         <v>2127</v>
       </c>
@@ -62960,6 +63563,9 @@
       <c r="C3208" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3208" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3208" s="1" t="s">
         <v>2129</v>
       </c>
@@ -62975,6 +63581,9 @@
       <c r="C3209" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3209" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3209" s="1" t="s">
         <v>1960</v>
       </c>
@@ -62990,6 +63599,9 @@
       <c r="C3210" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3210" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3210" s="1" t="s">
         <v>2130</v>
       </c>
@@ -63005,6 +63617,9 @@
       <c r="C3211" s="1" t="s">
         <v>1201</v>
       </c>
+      <c r="D3211" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3211" s="1" t="s">
         <v>2131</v>
       </c>
@@ -63020,6 +63635,9 @@
       <c r="C3212" s="1" t="s">
         <v>1201</v>
       </c>
+      <c r="D3212" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3212" s="1" t="s">
         <v>2132</v>
       </c>
@@ -63035,6 +63653,9 @@
       <c r="C3213" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="D3213" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3213" s="1" t="s">
         <v>2133</v>
       </c>
@@ -63050,6 +63671,9 @@
       <c r="C3214" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="D3214" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3214" s="1" t="s">
         <v>2134</v>
       </c>
@@ -63065,6 +63689,9 @@
       <c r="C3215" s="1" t="s">
         <v>175</v>
       </c>
+      <c r="D3215" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3215" s="1" t="s">
         <v>2135</v>
       </c>
@@ -63079,6 +63706,9 @@
       <c r="C3216" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="D3216" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3216" s="1" t="s">
         <v>2136</v>
       </c>
@@ -63093,6 +63723,9 @@
       <c r="C3217" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="D3217" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3217" s="1" t="s">
         <v>2137</v>
       </c>
@@ -63107,6 +63740,9 @@
       <c r="C3218" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="D3218" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3218" s="1" t="s">
         <v>2138</v>
       </c>
@@ -63121,6 +63757,9 @@
       <c r="C3219" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="D3219" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3219" s="1" t="s">
         <v>2139</v>
       </c>
@@ -63135,6 +63774,9 @@
       <c r="C3220" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3220" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3220" s="1" t="s">
         <v>772</v>
       </c>
@@ -63149,6 +63791,9 @@
       <c r="C3221" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3221" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3221" s="1" t="s">
         <v>10</v>
       </c>
@@ -63163,6 +63808,9 @@
       <c r="C3222" s="1" t="s">
         <v>1230</v>
       </c>
+      <c r="D3222" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3222" s="1" t="s">
         <v>2140</v>
       </c>
@@ -63177,6 +63825,9 @@
       <c r="C3223" s="1" t="s">
         <v>2142</v>
       </c>
+      <c r="D3223" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3223" s="1" t="s">
         <v>2141</v>
       </c>
@@ -63191,6 +63842,9 @@
       <c r="C3224" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3224" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3224" s="1" t="s">
         <v>10</v>
       </c>
@@ -63206,6 +63860,9 @@
       <c r="C3225" s="1" t="s">
         <v>1233</v>
       </c>
+      <c r="D3225" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3225" s="1" t="s">
         <v>2144</v>
       </c>
@@ -63221,6 +63878,9 @@
       <c r="C3226" s="1" t="s">
         <v>1168</v>
       </c>
+      <c r="D3226" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3226" s="1" t="s">
         <v>2145</v>
       </c>
@@ -63236,6 +63896,9 @@
       <c r="C3227" s="1" t="s">
         <v>1168</v>
       </c>
+      <c r="D3227" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3227" s="1" t="s">
         <v>2146</v>
       </c>
@@ -63250,6 +63913,9 @@
       <c r="C3228" s="1" t="s">
         <v>1149</v>
       </c>
+      <c r="D3228" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3228" s="1" t="s">
         <v>2147</v>
       </c>
@@ -63264,6 +63930,9 @@
       <c r="C3229" s="1" t="s">
         <v>2150</v>
       </c>
+      <c r="D3229" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3229" s="1" t="s">
         <v>2148</v>
       </c>
@@ -63278,6 +63947,9 @@
       <c r="C3230" s="1" t="s">
         <v>2153</v>
       </c>
+      <c r="D3230" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3230" s="1" t="s">
         <v>2151</v>
       </c>
@@ -63292,6 +63964,9 @@
       <c r="C3231" s="1" t="s">
         <v>2155</v>
       </c>
+      <c r="D3231" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3231" s="1" t="s">
         <v>2154</v>
       </c>
@@ -63306,6 +63981,9 @@
       <c r="C3232" s="1" t="s">
         <v>2158</v>
       </c>
+      <c r="D3232" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3232" s="1" t="s">
         <v>2156</v>
       </c>
@@ -63320,6 +63998,9 @@
       <c r="C3233" s="1" t="s">
         <v>2161</v>
       </c>
+      <c r="D3233" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3233" s="1" t="s">
         <v>2159</v>
       </c>
@@ -63334,6 +64015,9 @@
       <c r="C3234" s="1" t="s">
         <v>2164</v>
       </c>
+      <c r="D3234" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3234" s="1" t="s">
         <v>2162</v>
       </c>
@@ -63348,6 +64032,9 @@
       <c r="C3235" s="1" t="s">
         <v>2167</v>
       </c>
+      <c r="D3235" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3235" s="1" t="s">
         <v>2165</v>
       </c>
@@ -63362,6 +64049,9 @@
       <c r="C3236" s="1" t="s">
         <v>2170</v>
       </c>
+      <c r="D3236" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3236" s="1" t="s">
         <v>2168</v>
       </c>
@@ -63376,6 +64066,9 @@
       <c r="C3237" s="1" t="s">
         <v>2173</v>
       </c>
+      <c r="D3237" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3237" s="1" t="s">
         <v>2171</v>
       </c>
@@ -63390,6 +64083,9 @@
       <c r="C3238" s="1" t="s">
         <v>2176</v>
       </c>
+      <c r="D3238" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3238" s="1" t="s">
         <v>2174</v>
       </c>
@@ -63404,6 +64100,9 @@
       <c r="C3239" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3239" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3239" s="1" t="s">
         <v>2177</v>
       </c>
@@ -63418,6 +64117,9 @@
       <c r="C3240" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3240" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3240" s="1" t="s">
         <v>2178</v>
       </c>
@@ -63432,6 +64134,9 @@
       <c r="C3241" s="1" t="s">
         <v>2182</v>
       </c>
+      <c r="D3241" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3241" s="1" t="s">
         <v>2180</v>
       </c>
@@ -63446,6 +64151,9 @@
       <c r="C3242" s="1" t="s">
         <v>2185</v>
       </c>
+      <c r="D3242" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3242" s="1" t="s">
         <v>2183</v>
       </c>
@@ -63460,6 +64168,9 @@
       <c r="C3243" s="1" t="s">
         <v>2187</v>
       </c>
+      <c r="D3243" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3243" s="1" t="s">
         <v>2186</v>
       </c>
@@ -63474,6 +64185,9 @@
       <c r="C3244" s="1" t="s">
         <v>2190</v>
       </c>
+      <c r="D3244" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3244" s="1" t="s">
         <v>2188</v>
       </c>
@@ -63488,6 +64202,9 @@
       <c r="C3245" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3245" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3245" s="1" t="s">
         <v>1768</v>
       </c>
@@ -63502,6 +64219,9 @@
       <c r="C3246" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3246" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3246" s="1" t="s">
         <v>10</v>
       </c>
@@ -63517,6 +64237,9 @@
       <c r="C3247" s="1" t="s">
         <v>1482</v>
       </c>
+      <c r="D3247" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3247" s="1" t="s">
         <v>2192</v>
       </c>
@@ -63532,6 +64255,9 @@
       <c r="C3248" s="1" t="s">
         <v>1490</v>
       </c>
+      <c r="D3248" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3248" s="1" t="s">
         <v>2194</v>
       </c>
@@ -63546,6 +64272,9 @@
       <c r="C3249" s="1" t="s">
         <v>1495</v>
       </c>
+      <c r="D3249" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3249" s="1" t="s">
         <v>2195</v>
       </c>
@@ -63560,6 +64289,9 @@
       <c r="C3250" s="1" t="s">
         <v>1503</v>
       </c>
+      <c r="D3250" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3250" s="1" t="s">
         <v>2197</v>
       </c>
@@ -63574,6 +64306,9 @@
       <c r="C3251" s="1" t="s">
         <v>1507</v>
       </c>
+      <c r="D3251" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3251" s="1" t="s">
         <v>2192</v>
       </c>
@@ -63588,6 +64323,9 @@
       <c r="C3252" s="1" t="s">
         <v>1517</v>
       </c>
+      <c r="D3252" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3252" s="1" t="s">
         <v>2199</v>
       </c>
@@ -63602,6 +64340,9 @@
       <c r="C3253" s="1" t="s">
         <v>1521</v>
       </c>
+      <c r="D3253" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3253" s="1" t="s">
         <v>2201</v>
       </c>
@@ -63616,6 +64357,9 @@
       <c r="C3254" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3254" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3254" s="1" t="s">
         <v>10</v>
       </c>
@@ -63631,6 +64375,9 @@
       <c r="C3255" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3255" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3255" s="1" t="s">
         <v>10</v>
       </c>
@@ -63646,6 +64393,9 @@
       <c r="C3256" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3256" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3256" s="1" t="s">
         <v>2203</v>
       </c>
@@ -63661,6 +64411,9 @@
       <c r="C3257" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3257" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3257" s="1" t="s">
         <v>10</v>
       </c>
@@ -63676,6 +64429,9 @@
       <c r="C3258" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3258" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3258" s="1" t="s">
         <v>2204</v>
       </c>
@@ -63690,6 +64446,9 @@
       <c r="C3259" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3259" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3259" s="1" t="s">
         <v>2206</v>
       </c>
@@ -63705,6 +64464,9 @@
       <c r="C3260" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3260" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3260" s="1" t="s">
         <v>2208</v>
       </c>
@@ -63719,6 +64481,9 @@
       <c r="C3261" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3261" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3261" s="1" t="s">
         <v>2210</v>
       </c>
@@ -63733,6 +64498,9 @@
       <c r="C3262" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3262" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3262" s="1" t="s">
         <v>2211</v>
       </c>
@@ -63747,6 +64515,9 @@
       <c r="C3263" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3263" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3263" s="1" t="s">
         <v>2213</v>
       </c>
@@ -63761,6 +64532,9 @@
       <c r="C3264" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3264" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3264" s="1" t="s">
         <v>2215</v>
       </c>
@@ -63775,6 +64549,9 @@
       <c r="C3265" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3265" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3265" s="1" t="s">
         <v>2217</v>
       </c>
@@ -63789,6 +64566,9 @@
       <c r="C3266" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3266" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3266" s="1" t="s">
         <v>2219</v>
       </c>
@@ -63803,6 +64583,9 @@
       <c r="C3267" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3267" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3267" s="1" t="s">
         <v>2221</v>
       </c>
@@ -63817,6 +64600,9 @@
       <c r="C3268" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3268" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3268" s="1" t="s">
         <v>2223</v>
       </c>
@@ -63831,6 +64617,9 @@
       <c r="C3269" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3269" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3269" s="1" t="s">
         <v>2224</v>
       </c>
@@ -63845,6 +64634,9 @@
       <c r="C3270" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3270" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3270" s="1" t="s">
         <v>2225</v>
       </c>
@@ -63859,6 +64651,9 @@
       <c r="C3271" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3271" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3271" s="1" t="s">
         <v>2226</v>
       </c>
@@ -63873,6 +64668,9 @@
       <c r="C3272" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3272" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3272" s="1" t="s">
         <v>2227</v>
       </c>
@@ -63887,6 +64685,9 @@
       <c r="C3273" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3273" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3273" s="1" t="s">
         <v>2228</v>
       </c>
@@ -63901,6 +64702,9 @@
       <c r="C3274" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3274" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3274" s="1" t="s">
         <v>2229</v>
       </c>
@@ -63915,6 +64719,9 @@
       <c r="C3275" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3275" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3275" s="1" t="s">
         <v>2230</v>
       </c>
@@ -63930,6 +64737,9 @@
       <c r="C3276" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3276" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3276" s="1" t="s">
         <v>2231</v>
       </c>
@@ -63944,6 +64754,9 @@
       <c r="C3277" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3277" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3277" s="1" t="s">
         <v>2232</v>
       </c>
@@ -63958,6 +64771,9 @@
       <c r="C3278" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3278" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3278" s="1" t="s">
         <v>2233</v>
       </c>
@@ -63972,6 +64788,9 @@
       <c r="C3279" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3279" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3279" s="1" t="s">
         <v>2234</v>
       </c>
@@ -63986,6 +64805,9 @@
       <c r="C3280" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3280" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3280" s="1" t="s">
         <v>2235</v>
       </c>
@@ -64000,6 +64822,9 @@
       <c r="C3281" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3281" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3281" s="1" t="s">
         <v>2236</v>
       </c>
@@ -64014,6 +64839,9 @@
       <c r="C3282" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3282" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3282" s="1" t="s">
         <v>2237</v>
       </c>
@@ -64028,6 +64856,9 @@
       <c r="C3283" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3283" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3283" s="1" t="s">
         <v>2238</v>
       </c>
@@ -64042,6 +64873,9 @@
       <c r="C3284" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3284" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3284" s="1" t="s">
         <v>2239</v>
       </c>
@@ -64056,6 +64890,9 @@
       <c r="C3285" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3285" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3285" s="1" t="s">
         <v>2240</v>
       </c>
@@ -64070,6 +64907,9 @@
       <c r="C3286" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3286" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3286" s="1" t="s">
         <v>2241</v>
       </c>
@@ -64084,6 +64924,9 @@
       <c r="C3287" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3287" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3287" s="1" t="s">
         <v>2242</v>
       </c>
@@ -64098,6 +64941,9 @@
       <c r="C3288" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3288" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3288" s="1" t="s">
         <v>2243</v>
       </c>
@@ -64112,6 +64958,9 @@
       <c r="C3289" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3289" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3289" s="1" t="s">
         <v>2244</v>
       </c>
@@ -64126,6 +64975,9 @@
       <c r="C3290" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3290" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3290" s="1" t="s">
         <v>2245</v>
       </c>
@@ -64140,6 +64992,9 @@
       <c r="C3291" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3291" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3291" s="1" t="s">
         <v>2246</v>
       </c>
@@ -64154,6 +65009,9 @@
       <c r="C3292" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3292" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3292" s="1" t="s">
         <v>10</v>
       </c>
@@ -64168,6 +65026,9 @@
       <c r="C3293" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3293" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3293" s="1" t="s">
         <v>2247</v>
       </c>
@@ -64183,6 +65044,9 @@
       <c r="C3294" s="1" t="s">
         <v>2250</v>
       </c>
+      <c r="D3294" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3294" s="1" t="s">
         <v>2248</v>
       </c>
@@ -64198,6 +65062,9 @@
       <c r="C3295" s="1" t="s">
         <v>1972</v>
       </c>
+      <c r="D3295" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3295" s="1" t="s">
         <v>2251</v>
       </c>
@@ -64212,6 +65079,9 @@
       <c r="C3296" s="1" t="s">
         <v>1529</v>
       </c>
+      <c r="D3296" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3296" s="1" t="s">
         <v>2253</v>
       </c>
@@ -64226,6 +65096,9 @@
       <c r="C3297" s="1" t="s">
         <v>1533</v>
       </c>
+      <c r="D3297" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3297" s="1" t="s">
         <v>2255</v>
       </c>
@@ -64240,6 +65113,9 @@
       <c r="C3298" s="1" t="s">
         <v>1537</v>
       </c>
+      <c r="D3298" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3298" s="1" t="s">
         <v>2257</v>
       </c>
@@ -64271,6 +65147,9 @@
       <c r="C3300" s="1" t="s">
         <v>1549</v>
       </c>
+      <c r="D3300" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3300" s="1" t="s">
         <v>2262</v>
       </c>
@@ -64285,6 +65164,9 @@
       <c r="C3301" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3301" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3301" s="1" t="s">
         <v>2263</v>
       </c>
@@ -64299,6 +65181,9 @@
       <c r="C3302" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3302" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3302" s="1" t="s">
         <v>2265</v>
       </c>
@@ -64313,6 +65198,9 @@
       <c r="C3303" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3303" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3303" s="1" t="s">
         <v>2267</v>
       </c>
@@ -64328,6 +65216,9 @@
       <c r="C3304" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3304" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3304" s="1" t="s">
         <v>10</v>
       </c>
@@ -64342,6 +65233,9 @@
       <c r="C3305" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="D3305" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3305" s="1" t="s">
         <v>2269</v>
       </c>
@@ -64356,6 +65250,9 @@
       <c r="C3306" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3306" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3306" s="1" t="s">
         <v>10</v>
       </c>
@@ -64370,6 +65267,9 @@
       <c r="C3307" s="1" t="s">
         <v>1331</v>
       </c>
+      <c r="D3307" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3307" s="1" t="s">
         <v>2271</v>
       </c>
@@ -64401,6 +65301,9 @@
       <c r="C3309" s="1" t="s">
         <v>2275</v>
       </c>
+      <c r="D3309" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3309" s="1" t="s">
         <v>10</v>
       </c>
@@ -64415,6 +65318,9 @@
       <c r="C3310" s="1" t="s">
         <v>1327</v>
       </c>
+      <c r="D3310" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3310" s="1" t="s">
         <v>2276</v>
       </c>
@@ -64429,6 +65335,9 @@
       <c r="C3311" s="1" t="s">
         <v>1972</v>
       </c>
+      <c r="D3311" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3311" s="1" t="s">
         <v>2277</v>
       </c>
@@ -64460,6 +65369,9 @@
       <c r="C3313" s="1" t="s">
         <v>1537</v>
       </c>
+      <c r="D3313" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3313" s="1" t="s">
         <v>2282</v>
       </c>
@@ -64474,6 +65386,9 @@
       <c r="C3314" s="1" t="s">
         <v>1544</v>
       </c>
+      <c r="D3314" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3314" s="1" t="s">
         <v>2284</v>
       </c>
@@ -64488,6 +65403,9 @@
       <c r="C3315" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3315" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3315" s="1" t="s">
         <v>2285</v>
       </c>
@@ -64503,6 +65421,9 @@
       <c r="C3316" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3316" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3316" s="1" t="s">
         <v>2287</v>
       </c>
@@ -64518,6 +65439,9 @@
       <c r="C3317" s="1" t="s">
         <v>1308</v>
       </c>
+      <c r="D3317" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3317" s="1" t="s">
         <v>2289</v>
       </c>
@@ -64533,6 +65457,9 @@
       <c r="C3318" s="1" t="s">
         <v>1310</v>
       </c>
+      <c r="D3318" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3318" s="1" t="s">
         <v>2291</v>
       </c>
@@ -64547,6 +65474,9 @@
       <c r="C3319" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="D3319" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3319" s="1" t="s">
         <v>2292</v>
       </c>
@@ -64561,6 +65491,9 @@
       <c r="C3320" s="1" t="s">
         <v>1331</v>
       </c>
+      <c r="D3320" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3320" s="1" t="s">
         <v>2294</v>
       </c>
@@ -64575,6 +65508,9 @@
       <c r="C3321" s="1" t="s">
         <v>1318</v>
       </c>
+      <c r="D3321" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3321" s="1" t="s">
         <v>2296</v>
       </c>
@@ -64589,6 +65525,9 @@
       <c r="C3322" s="1" t="s">
         <v>1325</v>
       </c>
+      <c r="D3322" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3322" s="1" t="s">
         <v>2297</v>
       </c>
@@ -64603,6 +65542,9 @@
       <c r="C3323" s="1" t="s">
         <v>1327</v>
       </c>
+      <c r="D3323" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3323" s="1" t="s">
         <v>2299</v>
       </c>
@@ -64617,6 +65559,9 @@
       <c r="C3324" s="1" t="s">
         <v>1482</v>
       </c>
+      <c r="D3324" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3324" s="1" t="s">
         <v>2300</v>
       </c>
@@ -64631,6 +65576,9 @@
       <c r="C3325" s="1" t="s">
         <v>1490</v>
       </c>
+      <c r="D3325" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3325" s="1" t="s">
         <v>2301</v>
       </c>
@@ -64645,6 +65593,9 @@
       <c r="C3326" s="1" t="s">
         <v>1495</v>
       </c>
+      <c r="D3326" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3326" s="1" t="s">
         <v>2303</v>
       </c>
@@ -64659,6 +65610,9 @@
       <c r="C3327" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3327" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3327" s="1" t="s">
         <v>2305</v>
       </c>
@@ -64673,6 +65627,9 @@
       <c r="C3328" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3328" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3328" s="1" t="s">
         <v>2307</v>
       </c>
@@ -64688,6 +65645,9 @@
       <c r="C3329" s="1" t="s">
         <v>1511</v>
       </c>
+      <c r="D3329" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3329" s="1" t="s">
         <v>2308</v>
       </c>
@@ -64702,6 +65662,9 @@
       <c r="C3330" s="1" t="s">
         <v>1517</v>
       </c>
+      <c r="D3330" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3330" s="1" t="s">
         <v>2310</v>
       </c>
@@ -64716,6 +65679,9 @@
       <c r="C3331" s="1" t="s">
         <v>1521</v>
       </c>
+      <c r="D3331" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3331" s="1" t="s">
         <v>2311</v>
       </c>
@@ -64731,6 +65697,9 @@
       <c r="C3332" s="1" t="s">
         <v>2315</v>
       </c>
+      <c r="D3332" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3332" s="1" t="s">
         <v>2313</v>
       </c>
@@ -64745,6 +65714,9 @@
       <c r="C3333" s="1" t="s">
         <v>1524</v>
       </c>
+      <c r="D3333" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3333" s="1" t="s">
         <v>2316</v>
       </c>
@@ -64760,6 +65732,9 @@
       <c r="C3334" s="1" t="s">
         <v>1544</v>
       </c>
+      <c r="D3334" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3334" s="1" t="s">
         <v>2318</v>
       </c>
@@ -64775,6 +65750,9 @@
       <c r="C3335" s="1" t="s">
         <v>1549</v>
       </c>
+      <c r="D3335" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3335" s="1" t="s">
         <v>2319</v>
       </c>
@@ -64789,6 +65767,9 @@
       <c r="C3336" s="1" t="s">
         <v>1312</v>
       </c>
+      <c r="D3336" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3336" s="1" t="s">
         <v>2320</v>
       </c>
@@ -64803,6 +65784,9 @@
       <c r="C3337" s="1" t="s">
         <v>1972</v>
       </c>
+      <c r="D3337" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3337" s="1" t="s">
         <v>2321</v>
       </c>
@@ -64817,6 +65801,9 @@
       <c r="C3338" s="1" t="s">
         <v>1533</v>
       </c>
+      <c r="D3338" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3338" s="1" t="s">
         <v>2323</v>
       </c>
@@ -64831,6 +65818,9 @@
       <c r="C3339" s="1" t="s">
         <v>1537</v>
       </c>
+      <c r="D3339" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3339" s="1" t="s">
         <v>2325</v>
       </c>
@@ -64845,6 +65835,9 @@
       <c r="C3340" s="1" t="s">
         <v>1544</v>
       </c>
+      <c r="D3340" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3340" s="1" t="s">
         <v>2327</v>
       </c>
@@ -64859,6 +65852,9 @@
       <c r="C3341" s="1" t="s">
         <v>1549</v>
       </c>
+      <c r="D3341" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3341" s="1" t="s">
         <v>2329</v>
       </c>
@@ -64890,6 +65886,9 @@
       <c r="C3343" s="1" t="s">
         <v>1308</v>
       </c>
+      <c r="D3343" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3343" s="1" t="s">
         <v>2334</v>
       </c>
@@ -64904,6 +65903,9 @@
       <c r="C3344" s="1" t="s">
         <v>1310</v>
       </c>
+      <c r="D3344" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3344" s="1" t="s">
         <v>2336</v>
       </c>
@@ -64918,6 +65920,9 @@
       <c r="C3345" s="1" t="s">
         <v>1314</v>
       </c>
+      <c r="D3345" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3345" s="1" t="s">
         <v>2338</v>
       </c>
@@ -64932,6 +65937,9 @@
       <c r="C3346" s="1" t="s">
         <v>1331</v>
       </c>
+      <c r="D3346" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3346" s="1" t="s">
         <v>2340</v>
       </c>
@@ -64946,6 +65954,9 @@
       <c r="C3347" s="1" t="s">
         <v>1318</v>
       </c>
+      <c r="D3347" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3347" s="1" t="s">
         <v>2342</v>
       </c>
@@ -64960,6 +65971,9 @@
       <c r="C3348" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3348" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3348" s="1" t="s">
         <v>2344</v>
       </c>
@@ -64974,6 +65988,9 @@
       <c r="C3349" s="1" t="s">
         <v>1327</v>
       </c>
+      <c r="D3349" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3349" s="1" t="s">
         <v>2345</v>
       </c>
@@ -64988,6 +66005,9 @@
       <c r="C3350" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3350" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3350" s="1" t="s">
         <v>10</v>
       </c>
@@ -65002,6 +66022,9 @@
       <c r="C3351" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3351" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3351" s="1" t="s">
         <v>445</v>
       </c>
@@ -65016,6 +66039,9 @@
       <c r="C3352" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3352" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3352" s="1" t="s">
         <v>445</v>
       </c>
@@ -65031,6 +66057,9 @@
       <c r="C3353" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3353" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3353" s="1" t="s">
         <v>445</v>
       </c>
@@ -65045,6 +66074,9 @@
       <c r="C3354" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3354" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3354" s="1" t="s">
         <v>445</v>
       </c>
@@ -65059,6 +66091,9 @@
       <c r="C3355" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3355" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3355" s="1" t="s">
         <v>2351</v>
       </c>
@@ -65073,6 +66108,9 @@
       <c r="C3356" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3356" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3356" s="1" t="s">
         <v>2353</v>
       </c>
@@ -65087,6 +66125,9 @@
       <c r="C3357" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3357" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3357" s="1" t="s">
         <v>2355</v>
       </c>
@@ -65101,6 +66142,9 @@
       <c r="C3358" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3358" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3358" s="1" t="s">
         <v>10</v>
       </c>
@@ -65115,6 +66159,9 @@
       <c r="C3359" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3359" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3359" s="1" t="s">
         <v>2357</v>
       </c>
@@ -65129,6 +66176,9 @@
       <c r="C3360" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3360" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3360" s="1" t="s">
         <v>2358</v>
       </c>
@@ -65143,6 +66193,9 @@
       <c r="C3361" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3361" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3361" s="1" t="s">
         <v>2359</v>
       </c>
@@ -65157,6 +66210,9 @@
       <c r="C3362" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3362" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3362" s="1" t="s">
         <v>2360</v>
       </c>
@@ -65171,6 +66227,9 @@
       <c r="C3363" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3363" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3363" s="1" t="s">
         <v>10</v>
       </c>
@@ -65186,6 +66245,9 @@
       <c r="C3364" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3364" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3364" s="1" t="s">
         <v>10</v>
       </c>
@@ -65200,6 +66262,9 @@
       <c r="C3365" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3365" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3365" s="1" t="s">
         <v>10</v>
       </c>
@@ -65214,6 +66279,9 @@
       <c r="C3366" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3366" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3366" s="1" t="s">
         <v>2361</v>
       </c>
@@ -65228,6 +66296,9 @@
       <c r="C3367" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3367" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3367" s="1" t="s">
         <v>2362</v>
       </c>
@@ -65242,6 +66313,9 @@
       <c r="C3368" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3368" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3368" s="1" t="s">
         <v>10</v>
       </c>
@@ -65256,6 +66330,9 @@
       <c r="C3369" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3369" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3369" s="1" t="s">
         <v>2363</v>
       </c>
@@ -65271,6 +66348,9 @@
       <c r="C3370" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3370" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3370" s="1" t="s">
         <v>10</v>
       </c>
@@ -65285,6 +66365,9 @@
       <c r="C3371" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3371" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3371" s="1" t="s">
         <v>445</v>
       </c>
@@ -65299,6 +66382,9 @@
       <c r="C3372" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3372" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3372" s="1" t="s">
         <v>2364</v>
       </c>
@@ -65313,6 +66399,9 @@
       <c r="C3373" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3373" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3373" s="1" t="s">
         <v>2365</v>
       </c>
@@ -65327,6 +66416,9 @@
       <c r="C3374" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3374" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3374" s="1" t="s">
         <v>2366</v>
       </c>
@@ -65341,6 +66433,9 @@
       <c r="C3375" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3375" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3375" s="1" t="s">
         <v>2367</v>
       </c>
@@ -65355,6 +66450,9 @@
       <c r="C3376" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3376" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3376" s="1" t="s">
         <v>445</v>
       </c>
@@ -65369,6 +66467,9 @@
       <c r="C3377" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3377" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3377" s="1" t="s">
         <v>10</v>
       </c>
@@ -65383,6 +66484,9 @@
       <c r="C3378" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3378" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3378" s="1" t="s">
         <v>2368</v>
       </c>
@@ -65397,6 +66501,9 @@
       <c r="C3379" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3379" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3379" s="1" t="s">
         <v>2369</v>
       </c>
@@ -65411,6 +66518,9 @@
       <c r="C3380" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3380" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3380" s="1" t="s">
         <v>2370</v>
       </c>
@@ -65425,6 +66535,9 @@
       <c r="C3381" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3381" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3381" s="1" t="s">
         <v>2372</v>
       </c>
@@ -65439,6 +66552,9 @@
       <c r="C3382" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3382" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3382" s="1" t="s">
         <v>2374</v>
       </c>
@@ -65453,6 +66569,9 @@
       <c r="C3383" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3383" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3383" s="1" t="s">
         <v>2375</v>
       </c>
@@ -65467,6 +66586,9 @@
       <c r="C3384" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3384" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3384" s="1" t="s">
         <v>2376</v>
       </c>
@@ -65481,6 +66603,9 @@
       <c r="C3385" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3385" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3385" s="1" t="s">
         <v>2377</v>
       </c>
@@ -65495,6 +66620,9 @@
       <c r="C3386" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3386" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3386" s="1" t="s">
         <v>2379</v>
       </c>
@@ -65509,6 +66637,9 @@
       <c r="C3387" s="1" t="s">
         <v>2383</v>
       </c>
+      <c r="D3387" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3387" s="1" t="s">
         <v>2381</v>
       </c>
@@ -65523,6 +66654,9 @@
       <c r="C3388" s="1" t="s">
         <v>2386</v>
       </c>
+      <c r="D3388" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3388" s="1" t="s">
         <v>2384</v>
       </c>
@@ -65537,6 +66671,9 @@
       <c r="C3389" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3389" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3389" s="1" t="s">
         <v>2387</v>
       </c>
@@ -65551,6 +66688,9 @@
       <c r="C3390" s="1" t="s">
         <v>1541</v>
       </c>
+      <c r="D3390" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3390" s="1" t="s">
         <v>2389</v>
       </c>
@@ -65565,6 +66705,9 @@
       <c r="C3391" s="1" t="s">
         <v>1312</v>
       </c>
+      <c r="D3391" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3391" s="1" t="s">
         <v>2391</v>
       </c>
@@ -65579,6 +66722,9 @@
       <c r="C3392" s="1" t="s">
         <v>1889</v>
       </c>
+      <c r="D3392" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3392" s="1" t="s">
         <v>2393</v>
       </c>
@@ -65594,6 +66740,9 @@
       <c r="C3393" s="1" t="s">
         <v>2397</v>
       </c>
+      <c r="D3393" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3393" s="1" t="s">
         <v>2395</v>
       </c>
@@ -65609,6 +66758,9 @@
       <c r="C3394" s="1" t="s">
         <v>1500</v>
       </c>
+      <c r="D3394" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3394" s="1" t="s">
         <v>2398</v>
       </c>
@@ -65623,6 +66775,9 @@
       <c r="C3395" s="1" t="s">
         <v>2315</v>
       </c>
+      <c r="D3395" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3395" s="1" t="s">
         <v>2400</v>
       </c>
@@ -65637,6 +66792,9 @@
       <c r="C3396" s="1" t="s">
         <v>1331</v>
       </c>
+      <c r="D3396" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3396" s="1" t="s">
         <v>2402</v>
       </c>
@@ -65651,6 +66809,9 @@
       <c r="C3397" s="1" t="s">
         <v>1325</v>
       </c>
+      <c r="D3397" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3397" s="1" t="s">
         <v>2403</v>
       </c>
@@ -65665,6 +66826,9 @@
       <c r="C3398" s="1" t="s">
         <v>1541</v>
       </c>
+      <c r="D3398" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3398" s="1" t="s">
         <v>2404</v>
       </c>
@@ -65679,6 +66843,9 @@
       <c r="C3399" s="1" t="s">
         <v>1312</v>
       </c>
+      <c r="D3399" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3399" s="1" t="s">
         <v>2405</v>
       </c>
@@ -65694,6 +66861,9 @@
       <c r="C3400" s="1" t="s">
         <v>1889</v>
       </c>
+      <c r="D3400" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3400" s="1" t="s">
         <v>2407</v>
       </c>
@@ -65708,6 +66878,9 @@
       <c r="C3401" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3401" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3401" s="1" t="s">
         <v>10</v>
       </c>
@@ -65722,6 +66895,9 @@
       <c r="C3402" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3402" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3402" s="1" t="s">
         <v>10</v>
       </c>
@@ -65736,6 +66912,9 @@
       <c r="C3403" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3403" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3403" s="1" t="s">
         <v>10</v>
       </c>
@@ -65750,6 +66929,9 @@
       <c r="C3404" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3404" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3404" s="1" t="s">
         <v>10</v>
       </c>
@@ -65764,6 +66946,9 @@
       <c r="C3405" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3405" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3405" s="1" t="s">
         <v>10</v>
       </c>
@@ -65778,6 +66963,9 @@
       <c r="C3406" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3406" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3406" s="1" t="s">
         <v>10</v>
       </c>
@@ -65792,6 +66980,9 @@
       <c r="C3407" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3407" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3407" s="1" t="s">
         <v>2409</v>
       </c>
@@ -65806,6 +66997,9 @@
       <c r="C3408" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3408" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3408" s="1" t="s">
         <v>10</v>
       </c>
@@ -65820,6 +67014,9 @@
       <c r="C3409" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3409" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3409" s="1" t="s">
         <v>10</v>
       </c>
@@ -65835,6 +67032,9 @@
       <c r="C3410" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3410" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3410" s="1" t="s">
         <v>10</v>
       </c>
@@ -65850,6 +67050,9 @@
       <c r="C3411" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3411" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3411" s="1" t="s">
         <v>10</v>
       </c>
@@ -65865,6 +67068,9 @@
       <c r="C3412" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3412" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3412" s="1" t="s">
         <v>2410</v>
       </c>
@@ -65879,6 +67085,9 @@
       <c r="C3413" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3413" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3413" s="1" t="s">
         <v>10</v>
       </c>
@@ -65893,6 +67102,9 @@
       <c r="C3414" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3414" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3414" s="1" t="s">
         <v>10</v>
       </c>
@@ -65907,6 +67119,9 @@
       <c r="C3415" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3415" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3415" s="1" t="s">
         <v>10</v>
       </c>
@@ -65922,6 +67137,9 @@
       <c r="C3416" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3416" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3416" s="1" t="s">
         <v>10</v>
       </c>
@@ -65936,6 +67154,9 @@
       <c r="C3417" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3417" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3417" s="1" t="s">
         <v>10</v>
       </c>
@@ -65950,6 +67171,9 @@
       <c r="C3418" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3418" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3418" s="1" t="s">
         <v>10</v>
       </c>
@@ -65964,6 +67188,9 @@
       <c r="C3419" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3419" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3419" s="1" t="s">
         <v>10</v>
       </c>
@@ -65978,6 +67205,9 @@
       <c r="C3420" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3420" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3420" s="1" t="s">
         <v>10</v>
       </c>
@@ -65992,6 +67222,9 @@
       <c r="C3421" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3421" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3421" s="1" t="s">
         <v>10</v>
       </c>
@@ -66006,6 +67239,9 @@
       <c r="C3422" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3422" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3422" s="1" t="s">
         <v>10</v>
       </c>
@@ -66020,6 +67256,9 @@
       <c r="C3423" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3423" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3423" s="1" t="s">
         <v>10</v>
       </c>
@@ -66034,6 +67273,9 @@
       <c r="C3424" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3424" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3424" s="1" t="s">
         <v>10</v>
       </c>
@@ -66049,6 +67291,9 @@
       <c r="C3425" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3425" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3425" s="1" t="s">
         <v>10</v>
       </c>
@@ -66063,6 +67308,9 @@
       <c r="C3426" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3426" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3426" s="1" t="s">
         <v>10</v>
       </c>
@@ -66077,6 +67325,9 @@
       <c r="C3427" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3427" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3427" s="1" t="s">
         <v>10</v>
       </c>
@@ -66089,6 +67340,9 @@
         <v>10</v>
       </c>
       <c r="C3428" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3428" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3428" s="1" t="s">

</xml_diff>